<commit_message>
trimValues() option added for Excel parsers
</commit_message>
<xml_diff>
--- a/src/test/resources/import.xlsx
+++ b/src/test/resources/import.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">String val</t>
   </si>
   <si>
-    <t xml:space="preserve">3 String</t>
+    <t xml:space="preserve">3 String </t>
   </si>
   <si>
     <t xml:space="preserve">0.25</t>
@@ -415,12 +415,12 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.65"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>